<commit_message>
add feature delete exam
</commit_message>
<xml_diff>
--- a/src/config/excel/2.xlsx
+++ b/src/config/excel/2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320C5AE8-9F96-4270-8F3B-6B2391E0849E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91AF4D8-0611-490B-9DF8-D7C36650443B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3323" yWindow="3290" windowWidth="15951" windowHeight="8230" xr2:uid="{2F6EBE46-FFA3-42E0-971A-65BAE9437A39}"/>
+    <workbookView xWindow="-210" yWindow="720" windowWidth="7100" windowHeight="10401" xr2:uid="{2F6EBE46-FFA3-42E0-971A-65BAE9437A39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>x</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+  <si>
+    <t>examid</t>
+  </si>
+  <si>
+    <t>courseid</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>starttime</t>
+  </si>
+  <si>
+    <t>endtime</t>
+  </si>
+  <si>
+    <t>12:00Am</t>
+  </si>
+  <si>
+    <t>10:00Am</t>
+  </si>
+  <si>
+    <t>12:10Am</t>
+  </si>
+  <si>
+    <t>1/12/2000</t>
+  </si>
+  <si>
+    <t>1/1/2000</t>
+  </si>
+  <si>
+    <t>slot</t>
   </si>
 </sst>
 </file>
@@ -69,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,33 +419,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F046EB61-BE10-4508-9729-C93D412EBD8E}">
-  <dimension ref="A2:D4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="10.5" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>